<commit_message>
cash/credit deposit report with full functionality
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/TaxReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/TaxReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallo\OneDrive\Documents\SCHOOL STUFF\05 Summer 2021\Capstone\malloyethan11\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF30FB27-EE8C-4E61-BD00-14589048878B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89988779-7390-48AA-ADED-CB27929B5CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26835" yWindow="660" windowWidth="22980" windowHeight="13770" xr2:uid="{0F3C99C4-9686-4B89-98EB-786B08DFBAC1}"/>
+    <workbookView xWindow="-26490" yWindow="1005" windowWidth="22980" windowHeight="13770" xr2:uid="{BF68D7C4-44EC-4B04-8FCB-F44E7E46D93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18F36B5-1A36-4B68-862E-E55CF66745C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6E7C51-0918-42F8-B97F-33A0D5A92723}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1">
-        <v>44400.83966435185</v>
+        <v>44400.906770833331</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed divide by zero error. fixed variables not getting assigned values. made it so that the date on the report reflects the user-entered date, not the current date.
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/TaxReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/TaxReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016be9303c01b4f8/Documents/SCHOOL STUFF/05 Summer 2021/Capstone/malloyethan11/report_creation_program/report_creation_program/report_creation_program/bin/Debug/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02B30C96-8C0B-41E4-BC6E-F7BBA92A87F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8D332BB-72BC-409E-B4DF-54FBD0968B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31395" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{B94BFA2C-6E9B-429C-BE84-3FB2411B1D63}"/>
+    <workbookView xWindow="-25905" yWindow="1830" windowWidth="22980" windowHeight="13770" xr2:uid="{D042EC4A-AB02-46C7-96E6-23D189D5BEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7178DFC-0C30-4BFB-82E2-EB963FCC1376}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2CE0F8-5C13-40D5-B5B8-49032E53094E}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1">
-        <v>44410.884479166663</v>
+        <v>44393</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -498,13 +498,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>957.58</v>
       </c>
       <c r="D6">
-        <v>65535</v>
+        <v>47.879000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -512,13 +512,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>48829.65</v>
       </c>
       <c r="D7">
-        <v>65535</v>
+        <v>12207.4125</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -526,13 +526,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>900.81</v>
       </c>
       <c r="D8">
-        <v>65535</v>
+        <v>45.040499999999994</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>56.77</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -548,13 +548,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>957.57999999999993</v>
       </c>
       <c r="D10">
-        <v>65535</v>
+        <v>47.878999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -576,13 +576,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>585.45000000000005</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>585.45000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -590,13 +590,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>49201.78</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>49201.78</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>7.8</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>900.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>